<commit_message>
added registration feature and buttons for reg styles fine -- do need to cehck tiesheet imiidelty doesnt get addedd in genrated ittmeshee
</commit_message>
<xml_diff>
--- a/generated_timesheets/February_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/February_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -1306,17 +1306,17 @@
           <t>24-February-2025</t>
         </is>
       </c>
-      <c r="C34" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C34" s="10" t="inlineStr"/>
       <c r="D34" s="11" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E34" s="10" t="inlineStr"/>
+      <c r="E34" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F34" s="10" t="inlineStr"/>
       <c r="G34" s="10" t="inlineStr"/>
       <c r="H34" s="13" t="inlineStr">
@@ -1334,17 +1334,17 @@
           <t>25-February-2025</t>
         </is>
       </c>
-      <c r="C35" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C35" s="10" t="inlineStr"/>
       <c r="D35" s="11" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E35" s="10" t="inlineStr"/>
+      <c r="E35" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F35" s="10" t="inlineStr"/>
       <c r="G35" s="10" t="inlineStr"/>
       <c r="H35" s="13" t="inlineStr">
@@ -1362,17 +1362,17 @@
           <t>26-February-2025</t>
         </is>
       </c>
-      <c r="C36" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C36" s="10" t="inlineStr"/>
       <c r="D36" s="11" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E36" s="10" t="inlineStr"/>
+      <c r="E36" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F36" s="10" t="inlineStr"/>
       <c r="G36" s="10" t="inlineStr"/>
       <c r="H36" s="13" t="inlineStr">
@@ -1390,17 +1390,17 @@
           <t>27-February-2025</t>
         </is>
       </c>
-      <c r="C37" s="10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C37" s="10" t="inlineStr"/>
       <c r="D37" s="11" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E37" s="10" t="inlineStr"/>
+      <c r="E37" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
       <c r="F37" s="10" t="inlineStr"/>
       <c r="G37" s="10" t="inlineStr"/>
       <c r="H37" s="13" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="C41" s="18" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>16.0</t>
         </is>
       </c>
       <c r="D41" s="19" t="inlineStr">
@@ -1471,7 +1471,7 @@
       </c>
       <c r="E41" s="18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="F41" s="18" t="inlineStr">

</xml_diff>

<commit_message>
corect few changes in style
</commit_message>
<xml_diff>
--- a/generated_timesheets/February_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/February_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="DD - MMM - YYYY"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="DD - MMM - YYYY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -33,13 +34,16 @@
       <color rgb="00000000"/>
     </font>
     <font>
-      <color rgb="00FF0000"/>
-    </font>
-    <font>
+      <name val="Arial"/>
       <color rgb="00000000"/>
+      <sz val="12"/>
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="9">
@@ -114,69 +118,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -544,1071 +540,1111 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:H52"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="91" customWidth="1" min="2" max="2"/>
+    <col width="9" customWidth="1" min="3" max="3"/>
+    <col width="16" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="17" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="1" t="n"/>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="n"/>
+      <c r="G1" s="1" t="n"/>
+      <c r="H1" s="1" t="n"/>
+    </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>To engage Agile Co-Development and ICT Professional Services via 19024 bulk tender (PR230941)</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="3" t="n"/>
-      <c r="F2" s="4" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>To engage Agile Co-Development ICT Professional Services via 19024 bulk tender (PR230941)</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="4" t="n"/>
+      <c r="F2" s="5" t="inlineStr">
         <is>
           <t>Month/Year</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="6" t="inlineStr">
         <is>
           <t>February - 2025</t>
         </is>
       </c>
-      <c r="H2" s="5" t="n"/>
+      <c r="H2" s="6" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>PO Ref</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="6" t="inlineStr">
         <is>
           <t>GVT000ECI24000829</t>
         </is>
       </c>
-      <c r="C3" s="5" t="n"/>
-      <c r="D3" s="5" t="n"/>
-      <c r="E3" s="3" t="n"/>
-      <c r="F3" s="4" t="inlineStr">
+      <c r="C3" s="6" t="n"/>
+      <c r="D3" s="6" t="n"/>
+      <c r="E3" s="4" t="n"/>
+      <c r="F3" s="5" t="inlineStr">
         <is>
           <t>Contractor</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="7" t="inlineStr">
         <is>
           <t>PALO IT</t>
         </is>
       </c>
-      <c r="H3" s="5" t="n"/>
+      <c r="H3" s="7" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>PO Date</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>1 May 24 - 30 Apr 25</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="n"/>
-      <c r="D4" s="5" t="n"/>
-      <c r="E4" s="3" t="n"/>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>1 May 24 - 30</t>
+        </is>
+      </c>
+      <c r="C4" s="6" t="n"/>
+      <c r="D4" s="6" t="n"/>
+      <c r="E4" s="4" t="n"/>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n"/>
+      <c r="E5" s="1" t="n"/>
+      <c r="F5" s="1" t="n"/>
+      <c r="G5" s="1" t="n"/>
+      <c r="H5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>Shamik Guha Ray</t>
         </is>
       </c>
-      <c r="C6" s="7" t="n"/>
-      <c r="D6" s="7" t="n"/>
-      <c r="E6" s="3" t="n"/>
-      <c r="F6" s="4" t="inlineStr">
+      <c r="C6" s="9" t="n"/>
+      <c r="D6" s="9" t="n"/>
+      <c r="E6" s="4" t="n"/>
+      <c r="F6" s="5" t="inlineStr">
         <is>
           <t>Skill Level</t>
         </is>
       </c>
-      <c r="G6" s="5" t="inlineStr">
+      <c r="G6" s="6" t="inlineStr">
         <is>
           <t>Professional</t>
         </is>
       </c>
-      <c r="H6" s="7" t="n"/>
+      <c r="H6" s="9" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>Role Specialization</t>
         </is>
       </c>
-      <c r="B7" s="6" t="inlineStr">
+      <c r="B7" s="8" t="inlineStr">
         <is>
           <t>DevOps Engineer - II</t>
         </is>
       </c>
-      <c r="C7" s="7" t="n"/>
-      <c r="D7" s="7" t="n"/>
-      <c r="E7" s="3" t="n"/>
+      <c r="C7" s="9" t="n"/>
+      <c r="D7" s="9" t="n"/>
+      <c r="E7" s="4" t="n"/>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" s="5" t="inlineStr">
         <is>
           <t>Group/Specialization</t>
         </is>
       </c>
-      <c r="B8" s="6" t="inlineStr">
+      <c r="B8" s="8" t="inlineStr">
         <is>
           <t>Consulting</t>
         </is>
       </c>
-      <c r="C8" s="7" t="n"/>
-      <c r="D8" s="7" t="n"/>
-      <c r="E8" s="3" t="n"/>
+      <c r="C8" s="9" t="n"/>
+      <c r="D8" s="9" t="n"/>
+      <c r="E8" s="4" t="n"/>
+      <c r="F8" s="1" t="n"/>
+      <c r="G8" s="1" t="n"/>
+      <c r="H8" s="1" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="n"/>
+      <c r="F9" s="1" t="n"/>
+      <c r="G9" s="1" t="n"/>
+      <c r="H9" s="1" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="inlineStr">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="10" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C10" s="9" t="inlineStr">
+      <c r="C10" s="11" t="inlineStr">
         <is>
           <t>At Work</t>
         </is>
       </c>
-      <c r="D10" s="10" t="inlineStr">
+      <c r="D10" s="12" t="inlineStr">
         <is>
           <t>Public Holiday</t>
         </is>
       </c>
-      <c r="E10" s="11" t="inlineStr">
+      <c r="E10" s="13" t="inlineStr">
         <is>
           <t>Sick Leave</t>
         </is>
       </c>
-      <c r="F10" s="8" t="inlineStr">
+      <c r="F10" s="10" t="inlineStr">
         <is>
           <t>Childcare Leave</t>
         </is>
       </c>
-      <c r="G10" s="12" t="inlineStr">
+      <c r="G10" s="14" t="inlineStr">
         <is>
           <t>Annual Leave</t>
         </is>
       </c>
-      <c r="H10" s="8" t="inlineStr">
+      <c r="H10" s="10" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="13" t="inlineStr">
+      <c r="A11" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="16" t="inlineStr">
         <is>
           <t>01-February-2025</t>
         </is>
       </c>
-      <c r="C11" s="14" t="inlineStr"/>
-      <c r="D11" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E11" s="14" t="inlineStr"/>
-      <c r="F11" s="14" t="inlineStr"/>
-      <c r="G11" s="14" t="inlineStr"/>
-      <c r="H11" s="16" t="inlineStr">
+      <c r="C11" s="17" t="inlineStr"/>
+      <c r="D11" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E11" s="17" t="inlineStr"/>
+      <c r="F11" s="17" t="inlineStr"/>
+      <c r="G11" s="17" t="inlineStr"/>
+      <c r="H11" s="19" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="15" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="13" t="inlineStr">
+      <c r="B12" s="16" t="inlineStr">
         <is>
           <t>02-February-2025</t>
         </is>
       </c>
-      <c r="C12" s="14" t="inlineStr"/>
-      <c r="D12" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E12" s="14" t="inlineStr"/>
-      <c r="F12" s="14" t="inlineStr"/>
-      <c r="G12" s="14" t="inlineStr"/>
-      <c r="H12" s="16" t="inlineStr">
+      <c r="C12" s="17" t="inlineStr"/>
+      <c r="D12" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E12" s="17" t="inlineStr"/>
+      <c r="F12" s="17" t="inlineStr"/>
+      <c r="G12" s="17" t="inlineStr"/>
+      <c r="H12" s="19" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="15" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="13" t="inlineStr">
+      <c r="B13" s="16" t="inlineStr">
         <is>
           <t>03-February-2025</t>
         </is>
       </c>
-      <c r="C13" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D13" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E13" s="14" t="inlineStr"/>
-      <c r="F13" s="14" t="inlineStr"/>
-      <c r="G13" s="14" t="inlineStr"/>
-      <c r="H13" s="17" t="inlineStr">
+      <c r="C13" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E13" s="17" t="inlineStr"/>
+      <c r="F13" s="17" t="inlineStr"/>
+      <c r="G13" s="17" t="inlineStr"/>
+      <c r="H13" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="13" t="n">
+      <c r="A14" s="15" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="13" t="inlineStr">
+      <c r="B14" s="16" t="inlineStr">
         <is>
           <t>04-February-2025</t>
         </is>
       </c>
-      <c r="C14" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D14" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E14" s="14" t="inlineStr"/>
-      <c r="F14" s="14" t="inlineStr"/>
-      <c r="G14" s="14" t="inlineStr"/>
-      <c r="H14" s="17" t="inlineStr">
+      <c r="C14" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E14" s="17" t="inlineStr"/>
+      <c r="F14" s="17" t="inlineStr"/>
+      <c r="G14" s="17" t="inlineStr"/>
+      <c r="H14" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="13" t="n">
+      <c r="A15" s="15" t="n">
         <v>5</v>
       </c>
-      <c r="B15" s="13" t="inlineStr">
+      <c r="B15" s="16" t="inlineStr">
         <is>
           <t>05-February-2025</t>
         </is>
       </c>
-      <c r="C15" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D15" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E15" s="14" t="inlineStr"/>
-      <c r="F15" s="14" t="inlineStr"/>
-      <c r="G15" s="14" t="inlineStr"/>
-      <c r="H15" s="17" t="inlineStr">
+      <c r="C15" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E15" s="17" t="inlineStr"/>
+      <c r="F15" s="17" t="inlineStr"/>
+      <c r="G15" s="17" t="inlineStr"/>
+      <c r="H15" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="13" t="n">
+      <c r="A16" s="15" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="13" t="inlineStr">
+      <c r="B16" s="16" t="inlineStr">
         <is>
           <t>06-February-2025</t>
         </is>
       </c>
-      <c r="C16" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D16" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E16" s="14" t="inlineStr"/>
-      <c r="F16" s="14" t="inlineStr"/>
-      <c r="G16" s="14" t="inlineStr"/>
-      <c r="H16" s="17" t="inlineStr">
+      <c r="C16" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E16" s="17" t="inlineStr"/>
+      <c r="F16" s="17" t="inlineStr"/>
+      <c r="G16" s="17" t="inlineStr"/>
+      <c r="H16" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="13" t="n">
+      <c r="A17" s="15" t="n">
         <v>7</v>
       </c>
-      <c r="B17" s="13" t="inlineStr">
+      <c r="B17" s="16" t="inlineStr">
         <is>
           <t>07-February-2025</t>
         </is>
       </c>
-      <c r="C17" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D17" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E17" s="14" t="inlineStr"/>
-      <c r="F17" s="14" t="inlineStr"/>
-      <c r="G17" s="14" t="inlineStr"/>
-      <c r="H17" s="17" t="inlineStr">
+      <c r="C17" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E17" s="17" t="inlineStr"/>
+      <c r="F17" s="17" t="inlineStr"/>
+      <c r="G17" s="17" t="inlineStr"/>
+      <c r="H17" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="13" t="n">
+      <c r="A18" s="15" t="n">
         <v>8</v>
       </c>
-      <c r="B18" s="13" t="inlineStr">
+      <c r="B18" s="16" t="inlineStr">
         <is>
           <t>08-February-2025</t>
         </is>
       </c>
-      <c r="C18" s="14" t="inlineStr"/>
-      <c r="D18" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E18" s="14" t="inlineStr"/>
-      <c r="F18" s="14" t="inlineStr"/>
-      <c r="G18" s="14" t="inlineStr"/>
-      <c r="H18" s="16" t="inlineStr">
+      <c r="C18" s="17" t="inlineStr"/>
+      <c r="D18" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" s="17" t="inlineStr"/>
+      <c r="F18" s="17" t="inlineStr"/>
+      <c r="G18" s="17" t="inlineStr"/>
+      <c r="H18" s="19" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="13" t="n">
+      <c r="A19" s="15" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="13" t="inlineStr">
+      <c r="B19" s="16" t="inlineStr">
         <is>
           <t>09-February-2025</t>
         </is>
       </c>
-      <c r="C19" s="14" t="inlineStr"/>
-      <c r="D19" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E19" s="14" t="inlineStr"/>
-      <c r="F19" s="14" t="inlineStr"/>
-      <c r="G19" s="14" t="inlineStr"/>
-      <c r="H19" s="16" t="inlineStr">
+      <c r="C19" s="17" t="inlineStr"/>
+      <c r="D19" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" s="17" t="inlineStr"/>
+      <c r="F19" s="17" t="inlineStr"/>
+      <c r="G19" s="17" t="inlineStr"/>
+      <c r="H19" s="19" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="13" t="n">
+      <c r="A20" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="B20" s="13" t="inlineStr">
+      <c r="B20" s="16" t="inlineStr">
         <is>
           <t>10-February-2025</t>
         </is>
       </c>
-      <c r="C20" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D20" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E20" s="14" t="inlineStr"/>
-      <c r="F20" s="14" t="inlineStr"/>
-      <c r="G20" s="14" t="inlineStr"/>
-      <c r="H20" s="17" t="inlineStr">
+      <c r="C20" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" s="17" t="inlineStr"/>
+      <c r="F20" s="17" t="inlineStr"/>
+      <c r="G20" s="17" t="inlineStr"/>
+      <c r="H20" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="13" t="n">
+      <c r="A21" s="15" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="13" t="inlineStr">
+      <c r="B21" s="16" t="inlineStr">
         <is>
           <t>11-February-2025</t>
         </is>
       </c>
-      <c r="C21" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D21" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E21" s="14" t="inlineStr"/>
-      <c r="F21" s="14" t="inlineStr"/>
-      <c r="G21" s="14" t="inlineStr"/>
-      <c r="H21" s="17" t="inlineStr">
+      <c r="C21" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="17" t="inlineStr"/>
+      <c r="F21" s="17" t="inlineStr"/>
+      <c r="G21" s="17" t="inlineStr"/>
+      <c r="H21" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="13" t="n">
+      <c r="A22" s="15" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="13" t="inlineStr">
+      <c r="B22" s="16" t="inlineStr">
         <is>
           <t>12-February-2025</t>
         </is>
       </c>
-      <c r="C22" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D22" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E22" s="14" t="inlineStr"/>
-      <c r="F22" s="14" t="inlineStr"/>
-      <c r="G22" s="14" t="inlineStr"/>
-      <c r="H22" s="17" t="inlineStr">
+      <c r="C22" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E22" s="17" t="inlineStr"/>
+      <c r="F22" s="17" t="inlineStr"/>
+      <c r="G22" s="17" t="inlineStr"/>
+      <c r="H22" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="13" t="n">
+      <c r="A23" s="15" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="13" t="inlineStr">
+      <c r="B23" s="16" t="inlineStr">
         <is>
           <t>13-February-2025</t>
         </is>
       </c>
-      <c r="C23" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D23" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E23" s="14" t="inlineStr"/>
-      <c r="F23" s="14" t="inlineStr"/>
-      <c r="G23" s="14" t="inlineStr"/>
-      <c r="H23" s="17" t="inlineStr">
+      <c r="C23" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" s="17" t="inlineStr"/>
+      <c r="F23" s="17" t="inlineStr"/>
+      <c r="G23" s="17" t="inlineStr"/>
+      <c r="H23" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="13" t="n">
+      <c r="A24" s="15" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="13" t="inlineStr">
+      <c r="B24" s="16" t="inlineStr">
         <is>
           <t>14-February-2025</t>
         </is>
       </c>
-      <c r="C24" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D24" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E24" s="14" t="inlineStr"/>
-      <c r="F24" s="14" t="inlineStr"/>
-      <c r="G24" s="14" t="inlineStr"/>
-      <c r="H24" s="17" t="inlineStr">
+      <c r="C24" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" s="17" t="inlineStr"/>
+      <c r="F24" s="17" t="inlineStr"/>
+      <c r="G24" s="17" t="inlineStr"/>
+      <c r="H24" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="13" t="n">
+      <c r="A25" s="15" t="n">
         <v>15</v>
       </c>
-      <c r="B25" s="13" t="inlineStr">
+      <c r="B25" s="16" t="inlineStr">
         <is>
           <t>15-February-2025</t>
         </is>
       </c>
-      <c r="C25" s="14" t="inlineStr"/>
-      <c r="D25" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E25" s="14" t="inlineStr"/>
-      <c r="F25" s="14" t="inlineStr"/>
-      <c r="G25" s="14" t="inlineStr"/>
-      <c r="H25" s="16" t="inlineStr">
+      <c r="C25" s="17" t="inlineStr"/>
+      <c r="D25" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" s="17" t="inlineStr"/>
+      <c r="F25" s="17" t="inlineStr"/>
+      <c r="G25" s="17" t="inlineStr"/>
+      <c r="H25" s="19" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="13" t="n">
+      <c r="A26" s="15" t="n">
         <v>16</v>
       </c>
-      <c r="B26" s="13" t="inlineStr">
+      <c r="B26" s="16" t="inlineStr">
         <is>
           <t>16-February-2025</t>
         </is>
       </c>
-      <c r="C26" s="14" t="inlineStr"/>
-      <c r="D26" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E26" s="14" t="inlineStr"/>
-      <c r="F26" s="14" t="inlineStr"/>
-      <c r="G26" s="14" t="inlineStr"/>
-      <c r="H26" s="16" t="inlineStr">
+      <c r="C26" s="17" t="inlineStr"/>
+      <c r="D26" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" s="17" t="inlineStr"/>
+      <c r="F26" s="17" t="inlineStr"/>
+      <c r="G26" s="17" t="inlineStr"/>
+      <c r="H26" s="19" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="13" t="n">
+      <c r="A27" s="15" t="n">
         <v>17</v>
       </c>
-      <c r="B27" s="13" t="inlineStr">
+      <c r="B27" s="16" t="inlineStr">
         <is>
           <t>17-February-2025</t>
         </is>
       </c>
-      <c r="C27" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D27" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E27" s="14" t="inlineStr"/>
-      <c r="F27" s="14" t="inlineStr"/>
-      <c r="G27" s="14" t="inlineStr"/>
-      <c r="H27" s="17" t="inlineStr">
+      <c r="C27" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E27" s="17" t="inlineStr"/>
+      <c r="F27" s="17" t="inlineStr"/>
+      <c r="G27" s="17" t="inlineStr"/>
+      <c r="H27" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="13" t="n">
+      <c r="A28" s="15" t="n">
         <v>18</v>
       </c>
-      <c r="B28" s="13" t="inlineStr">
+      <c r="B28" s="16" t="inlineStr">
         <is>
           <t>18-February-2025</t>
         </is>
       </c>
-      <c r="C28" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D28" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E28" s="14" t="inlineStr"/>
-      <c r="F28" s="14" t="inlineStr"/>
-      <c r="G28" s="14" t="inlineStr"/>
-      <c r="H28" s="17" t="inlineStr">
+      <c r="C28" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" s="17" t="inlineStr"/>
+      <c r="F28" s="17" t="inlineStr"/>
+      <c r="G28" s="17" t="inlineStr"/>
+      <c r="H28" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="13" t="n">
+      <c r="A29" s="15" t="n">
         <v>19</v>
       </c>
-      <c r="B29" s="13" t="inlineStr">
+      <c r="B29" s="16" t="inlineStr">
         <is>
           <t>19-February-2025</t>
         </is>
       </c>
-      <c r="C29" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D29" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E29" s="14" t="inlineStr"/>
-      <c r="F29" s="14" t="inlineStr"/>
-      <c r="G29" s="14" t="inlineStr"/>
-      <c r="H29" s="17" t="inlineStr">
+      <c r="C29" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" s="17" t="inlineStr"/>
+      <c r="F29" s="17" t="inlineStr"/>
+      <c r="G29" s="17" t="inlineStr"/>
+      <c r="H29" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="13" t="n">
+      <c r="A30" s="15" t="n">
         <v>20</v>
       </c>
-      <c r="B30" s="13" t="inlineStr">
+      <c r="B30" s="16" t="inlineStr">
         <is>
           <t>20-February-2025</t>
         </is>
       </c>
-      <c r="C30" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D30" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E30" s="14" t="inlineStr"/>
-      <c r="F30" s="14" t="inlineStr"/>
-      <c r="G30" s="14" t="inlineStr"/>
-      <c r="H30" s="17" t="inlineStr">
+      <c r="C30" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E30" s="17" t="inlineStr"/>
+      <c r="F30" s="17" t="inlineStr"/>
+      <c r="G30" s="17" t="inlineStr"/>
+      <c r="H30" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="13" t="n">
+      <c r="A31" s="15" t="n">
         <v>21</v>
       </c>
-      <c r="B31" s="13" t="inlineStr">
+      <c r="B31" s="16" t="inlineStr">
         <is>
           <t>21-February-2025</t>
         </is>
       </c>
-      <c r="C31" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D31" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E31" s="14" t="inlineStr"/>
-      <c r="F31" s="14" t="inlineStr"/>
-      <c r="G31" s="14" t="inlineStr"/>
-      <c r="H31" s="17" t="inlineStr">
+      <c r="C31" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" s="17" t="inlineStr"/>
+      <c r="F31" s="17" t="inlineStr"/>
+      <c r="G31" s="17" t="inlineStr"/>
+      <c r="H31" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="13" t="n">
+      <c r="A32" s="15" t="n">
         <v>22</v>
       </c>
-      <c r="B32" s="13" t="inlineStr">
+      <c r="B32" s="16" t="inlineStr">
         <is>
           <t>22-February-2025</t>
         </is>
       </c>
-      <c r="C32" s="14" t="inlineStr"/>
-      <c r="D32" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E32" s="14" t="inlineStr"/>
-      <c r="F32" s="14" t="inlineStr"/>
-      <c r="G32" s="14" t="inlineStr"/>
-      <c r="H32" s="16" t="inlineStr">
+      <c r="C32" s="17" t="inlineStr"/>
+      <c r="D32" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" s="17" t="inlineStr"/>
+      <c r="F32" s="17" t="inlineStr"/>
+      <c r="G32" s="17" t="inlineStr"/>
+      <c r="H32" s="19" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="13" t="n">
+      <c r="A33" s="15" t="n">
         <v>23</v>
       </c>
-      <c r="B33" s="13" t="inlineStr">
+      <c r="B33" s="16" t="inlineStr">
         <is>
           <t>23-February-2025</t>
         </is>
       </c>
-      <c r="C33" s="14" t="inlineStr"/>
-      <c r="D33" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E33" s="14" t="inlineStr"/>
-      <c r="F33" s="14" t="inlineStr"/>
-      <c r="G33" s="14" t="inlineStr"/>
-      <c r="H33" s="16" t="inlineStr">
+      <c r="C33" s="17" t="inlineStr"/>
+      <c r="D33" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" s="17" t="inlineStr"/>
+      <c r="F33" s="17" t="inlineStr"/>
+      <c r="G33" s="17" t="inlineStr"/>
+      <c r="H33" s="19" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="13" t="n">
+      <c r="A34" s="15" t="n">
         <v>24</v>
       </c>
-      <c r="B34" s="13" t="inlineStr">
+      <c r="B34" s="16" t="inlineStr">
         <is>
           <t>24-February-2025</t>
         </is>
       </c>
-      <c r="C34" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D34" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E34" s="14" t="inlineStr"/>
-      <c r="F34" s="14" t="inlineStr"/>
-      <c r="G34" s="14" t="inlineStr"/>
-      <c r="H34" s="17" t="inlineStr">
+      <c r="C34" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" s="17" t="inlineStr"/>
+      <c r="F34" s="17" t="inlineStr"/>
+      <c r="G34" s="17" t="inlineStr"/>
+      <c r="H34" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="13" t="n">
+      <c r="A35" s="15" t="n">
         <v>25</v>
       </c>
-      <c r="B35" s="13" t="inlineStr">
+      <c r="B35" s="16" t="inlineStr">
         <is>
           <t>25-February-2025</t>
         </is>
       </c>
-      <c r="C35" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D35" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E35" s="14" t="inlineStr"/>
-      <c r="F35" s="14" t="inlineStr"/>
-      <c r="G35" s="14" t="inlineStr"/>
-      <c r="H35" s="17" t="inlineStr">
+      <c r="C35" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" s="17" t="inlineStr"/>
+      <c r="F35" s="17" t="inlineStr"/>
+      <c r="G35" s="17" t="inlineStr"/>
+      <c r="H35" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="13" t="n">
+      <c r="A36" s="15" t="n">
         <v>26</v>
       </c>
-      <c r="B36" s="13" t="inlineStr">
+      <c r="B36" s="16" t="inlineStr">
         <is>
           <t>26-February-2025</t>
         </is>
       </c>
-      <c r="C36" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D36" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E36" s="14" t="inlineStr"/>
-      <c r="F36" s="14" t="inlineStr"/>
-      <c r="G36" s="14" t="inlineStr"/>
-      <c r="H36" s="17" t="inlineStr">
+      <c r="C36" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" s="17" t="inlineStr"/>
+      <c r="F36" s="17" t="inlineStr"/>
+      <c r="G36" s="17" t="inlineStr"/>
+      <c r="H36" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="13" t="n">
+      <c r="A37" s="15" t="n">
         <v>27</v>
       </c>
-      <c r="B37" s="13" t="inlineStr">
+      <c r="B37" s="16" t="inlineStr">
         <is>
           <t>27-February-2025</t>
         </is>
       </c>
-      <c r="C37" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D37" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E37" s="14" t="inlineStr"/>
-      <c r="F37" s="14" t="inlineStr"/>
-      <c r="G37" s="14" t="inlineStr"/>
-      <c r="H37" s="17" t="inlineStr">
+      <c r="C37" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" s="17" t="inlineStr"/>
+      <c r="F37" s="17" t="inlineStr"/>
+      <c r="G37" s="17" t="inlineStr"/>
+      <c r="H37" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="13" t="n">
+      <c r="A38" s="15" t="n">
         <v>28</v>
       </c>
-      <c r="B38" s="13" t="inlineStr">
+      <c r="B38" s="16" t="inlineStr">
         <is>
           <t>28-February-2025</t>
         </is>
       </c>
-      <c r="C38" s="14" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D38" s="15" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E38" s="14" t="inlineStr"/>
-      <c r="F38" s="14" t="inlineStr"/>
-      <c r="G38" s="14" t="inlineStr"/>
-      <c r="H38" s="17" t="inlineStr">
+      <c r="C38" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E38" s="17" t="inlineStr"/>
+      <c r="F38" s="17" t="inlineStr"/>
+      <c r="G38" s="17" t="inlineStr"/>
+      <c r="H38" s="20" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="H39" s="18" t="n"/>
+      <c r="A39" s="1" t="n"/>
+      <c r="B39" s="1" t="n"/>
+      <c r="C39" s="1" t="n"/>
+      <c r="D39" s="1" t="n"/>
+      <c r="E39" s="1" t="n"/>
+      <c r="F39" s="1" t="n"/>
+      <c r="G39" s="1" t="n"/>
+      <c r="H39" s="1" t="n"/>
     </row>
     <row r="40">
-      <c r="H40" s="18" t="n"/>
+      <c r="A40" s="1" t="n"/>
+      <c r="B40" s="1" t="n"/>
+      <c r="C40" s="1" t="n"/>
+      <c r="D40" s="1" t="n"/>
+      <c r="E40" s="1" t="n"/>
+      <c r="F40" s="1" t="n"/>
+      <c r="G40" s="1" t="n"/>
+      <c r="H40" s="1" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="19" t="inlineStr">
+      <c r="A41" s="15" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B41" s="4" t="n"/>
-      <c r="C41" s="20" t="inlineStr">
-        <is>
-          <t>20.0</t>
-        </is>
-      </c>
-      <c r="D41" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E41" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F41" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G41" s="20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H41" s="21" t="n"/>
+      <c r="B41" s="5" t="n"/>
+      <c r="C41" s="18" t="n">
+        <v>20</v>
+      </c>
+      <c r="D41" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E41" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F41" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G41" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H41" s="5" t="n"/>
     </row>
     <row r="42">
-      <c r="H42" s="18" t="n"/>
+      <c r="A42" s="1" t="n"/>
+      <c r="B42" s="1" t="n"/>
+      <c r="C42" s="1" t="n"/>
+      <c r="D42" s="1" t="n"/>
+      <c r="E42" s="1" t="n"/>
+      <c r="F42" s="1" t="n"/>
+      <c r="G42" s="1" t="n"/>
+      <c r="H42" s="1" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
+      <c r="A43" s="2" t="inlineStr">
         <is>
           <t>Officer</t>
         </is>
       </c>
-      <c r="B43" s="22" t="inlineStr">
+      <c r="B43" s="7" t="inlineStr">
         <is>
           <t>Shamik Guha Ray</t>
         </is>
       </c>
-      <c r="C43" s="22" t="n"/>
-      <c r="D43" s="22" t="n"/>
-      <c r="H43" s="18" t="n"/>
+      <c r="C43" s="7" t="n"/>
+      <c r="D43" s="7" t="n"/>
+      <c r="E43" s="1" t="n"/>
+      <c r="F43" s="1" t="n"/>
+      <c r="G43" s="1" t="n"/>
+      <c r="H43" s="1" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
+      <c r="A44" s="2" t="inlineStr">
         <is>
           <t>Signature</t>
         </is>
       </c>
-      <c r="B44" s="22" t="inlineStr">
+      <c r="B44" s="7" t="inlineStr">
         <is>
           <t>Shamik Guha Ray</t>
         </is>
       </c>
-      <c r="C44" s="22" t="n"/>
-      <c r="D44" s="22" t="n"/>
-      <c r="H44" s="18" t="n"/>
+      <c r="C44" s="7" t="n"/>
+      <c r="D44" s="7" t="n"/>
+      <c r="E44" s="1" t="n"/>
+      <c r="F44" s="1" t="n"/>
+      <c r="G44" s="1" t="n"/>
+      <c r="H44" s="1" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
+      <c r="A45" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B45" s="23" t="inlineStr">
+      <c r="B45" s="21" t="inlineStr">
         <is>
           <t>10 - Feb - 2025</t>
         </is>
       </c>
-      <c r="C45" s="22" t="n"/>
-      <c r="D45" s="22" t="n"/>
-      <c r="H45" s="18" t="n"/>
+      <c r="C45" s="7" t="n"/>
+      <c r="D45" s="7" t="n"/>
+      <c r="E45" s="1" t="n"/>
+      <c r="F45" s="1" t="n"/>
+      <c r="G45" s="1" t="n"/>
+      <c r="H45" s="1" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n"/>
-      <c r="B46" s="22" t="n"/>
-      <c r="C46" s="22" t="n"/>
-      <c r="D46" s="22" t="n"/>
-      <c r="H46" s="18" t="n"/>
+      <c r="A46" s="2" t="n"/>
+      <c r="B46" s="7" t="n"/>
+      <c r="C46" s="7" t="n"/>
+      <c r="D46" s="7" t="n"/>
+      <c r="E46" s="1" t="n"/>
+      <c r="F46" s="1" t="n"/>
+      <c r="G46" s="1" t="n"/>
+      <c r="H46" s="1" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
+      <c r="A47" s="2" t="inlineStr">
         <is>
           <t>Reporting Officer</t>
         </is>
       </c>
-      <c r="B47" s="22" t="inlineStr">
+      <c r="B47" s="7" t="inlineStr">
         <is>
           <t>Deepu Joseph</t>
         </is>
       </c>
-      <c r="C47" s="22" t="n"/>
-      <c r="D47" s="22" t="n"/>
-      <c r="H47" s="18" t="n"/>
+      <c r="C47" s="7" t="n"/>
+      <c r="D47" s="7" t="n"/>
+      <c r="E47" s="1" t="n"/>
+      <c r="F47" s="1" t="n"/>
+      <c r="G47" s="1" t="n"/>
+      <c r="H47" s="1" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
+      <c r="A48" s="2" t="inlineStr">
         <is>
           <t>Signature</t>
         </is>
       </c>
-      <c r="B48" s="22" t="inlineStr"/>
-      <c r="C48" s="22" t="n"/>
-      <c r="D48" s="22" t="n"/>
-      <c r="H48" s="18" t="n"/>
+      <c r="B48" s="7" t="inlineStr"/>
+      <c r="C48" s="7" t="n"/>
+      <c r="D48" s="7" t="n"/>
+      <c r="E48" s="1" t="n"/>
+      <c r="F48" s="1" t="n"/>
+      <c r="G48" s="1" t="n"/>
+      <c r="H48" s="1" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
+      <c r="A49" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B49" s="23" t="inlineStr"/>
-      <c r="C49" s="22" t="n"/>
-      <c r="D49" s="22" t="n"/>
-      <c r="H49" s="18" t="n"/>
-    </row>
-    <row r="50">
-      <c r="H50" s="18" t="n"/>
-    </row>
-    <row r="51">
-      <c r="H51" s="18" t="n"/>
-    </row>
-    <row r="52">
-      <c r="H52" s="18" t="n"/>
+      <c r="B49" s="21" t="inlineStr"/>
+      <c r="C49" s="7" t="n"/>
+      <c r="D49" s="7" t="n"/>
+      <c r="E49" s="1" t="n"/>
+      <c r="F49" s="1" t="n"/>
+      <c r="G49" s="1" t="n"/>
+      <c r="H49" s="1" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="15">

</xml_diff>